<commit_message>
-Added more logic for Shadow events.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/Shadow_Lookup_Table.xlsx
+++ b/DI_Timer_App/Shadow_Lookup_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80A4FE3-C8A4-47D3-B772-CF648BAA4021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9345102F-E016-4853-8E81-915C641F8010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
+    <workbookView xWindow="28830" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
-Fixed labeling on Shadow Wars row.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/Shadow_Lookup_Table.xlsx
+++ b/DI_Timer_App/Shadow_Lookup_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\fight\Documents\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9345102F-E016-4853-8E81-915C641F8010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61001AB-1F16-4068-9638-71F948775CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,10 +82,10 @@
     <t>Shadow Lottery 9PM</t>
   </si>
   <si>
-    <t>Shadow War 7PM</t>
-  </si>
-  <si>
     <t>Rite of Exile 8PM</t>
+  </si>
+  <si>
+    <t>Shadow War 6PM</t>
   </si>
 </sst>
 </file>
@@ -440,17 +440,17 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,64 +467,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Changed reference spreadsheets due to changes.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/Shadow_Lookup_Table.xlsx
+++ b/DI_Timer_App/Shadow_Lookup_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\fight\Documents\diablo_immortal_event_app\DI_Timer_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61001AB-1F16-4068-9638-71F948775CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F2A42B-FEF8-4420-A5F2-6C98C62F9F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{F68A42B3-28CA-4941-B9AB-48F8CCD3EE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>Raid the Vault 7PM</t>
   </si>
   <si>
-    <t>Shadow Assembly 6PM</t>
-  </si>
-  <si>
     <t>Battlegrounds 8AM</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Shadow War 6PM</t>
+  </si>
+  <si>
+    <t>Shadow Assembly 7PM</t>
   </si>
 </sst>
 </file>
@@ -440,17 +440,17 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,64 +467,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>